<commit_message>
Added file for storing color thresholds, added xlsx for analyzing colors, added io_vision file which applies all masks done so far.
</commit_message>
<xml_diff>
--- a/color_analysis.xlsx
+++ b/color_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aidan\Documents\git_repos\genetic_paperIO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{EEA1A84E-97D9-4A7A-8725-6AC8BFBC1AD8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2A95CD8C-BB84-4518-B70E-779992D21A75}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="12225" xr2:uid="{921898DB-0026-4A37-B7E4-80C4136EB8F8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="11">
   <si>
     <t>Background</t>
   </si>
@@ -49,6 +49,15 @@
   </si>
   <si>
     <t>OpenCV Scale</t>
+  </si>
+  <si>
+    <t>Exact?</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -92,7 +101,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -101,6 +110,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -417,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A8A2413-EE7C-4011-93FC-BB63178B7FA7}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,7 +440,7 @@
     <col min="1" max="1" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>6</v>
       </c>
@@ -440,7 +452,7 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
@@ -459,8 +471,11 @@
       <c r="G2" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -485,8 +500,11 @@
         <f>(D3/100) * 255</f>
         <v>244.79999999999998</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -511,8 +529,11 @@
         <f t="shared" ref="G4:G5" si="2">(D4/100) * 255</f>
         <v>155.54999999999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -537,38 +558,191 @@
         <f t="shared" si="2"/>
         <v>249.9</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <f t="shared" ref="E6:E15" si="3">(B6/360) * 179</f>
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ref="F6:F15" si="4">(C6/100) * 255</f>
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <f t="shared" ref="G6:G15" si="5">(D6/100) * 255</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added grid detection and slicing
</commit_message>
<xml_diff>
--- a/color_analysis.xlsx
+++ b/color_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aidan\Documents\git_repos\genetic_paperIO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2A95CD8C-BB84-4518-B70E-779992D21A75}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5CE740EA-C7B8-4717-982B-3A1854A64BE7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="12225" xr2:uid="{921898DB-0026-4A37-B7E4-80C4136EB8F8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="12">
   <si>
     <t>Background</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>Yellow Area</t>
   </si>
 </sst>
 </file>
@@ -109,10 +112,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -432,7 +435,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,16 +444,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
@@ -500,7 +503,7 @@
         <f>(D3/100) * 255</f>
         <v>244.79999999999998</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -529,7 +532,7 @@
         <f t="shared" ref="G4:G5" si="2">(D4/100) * 255</f>
         <v>155.54999999999998</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -558,7 +561,7 @@
         <f t="shared" si="2"/>
         <v>249.9</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -576,25 +579,36 @@
         <f t="shared" ref="G6:G15" si="5">(D6/100) * 255</f>
         <v>0</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>60</v>
+      </c>
+      <c r="C7">
+        <v>79</v>
+      </c>
+      <c r="D7">
+        <v>83</v>
+      </c>
       <c r="E7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>29.833333333333332</v>
       </c>
       <c r="F7">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>201.45000000000002</v>
       </c>
       <c r="G7">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H7" s="4" t="s">
+        <v>211.64999999999998</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -612,7 +626,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -630,7 +644,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -648,7 +662,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -666,7 +680,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -684,7 +698,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H12" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -702,7 +716,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H13" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -720,7 +734,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -738,7 +752,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="H15" s="3" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Hue Buckets, they almost work.
</commit_message>
<xml_diff>
--- a/color_analysis.xlsx
+++ b/color_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aidan\Documents\git_repos\genetic_paperIO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5CE740EA-C7B8-4717-982B-3A1854A64BE7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8C49FBD1-475E-4CA4-AC0B-8585869C0FB0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="12225" xr2:uid="{921898DB-0026-4A37-B7E4-80C4136EB8F8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
   <si>
     <t>Background</t>
   </si>
@@ -61,6 +61,27 @@
   </si>
   <si>
     <t>Yellow Area</t>
+  </si>
+  <si>
+    <t>Pink Area</t>
+  </si>
+  <si>
+    <t>Pink Trail</t>
+  </si>
+  <si>
+    <t>Pink Person</t>
+  </si>
+  <si>
+    <t>Orange Area</t>
+  </si>
+  <si>
+    <t>Orange Trail</t>
+  </si>
+  <si>
+    <t>Orange Person</t>
+  </si>
+  <si>
+    <t>q</t>
   </si>
 </sst>
 </file>
@@ -435,7 +456,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,108 +634,174 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>298</v>
+      </c>
+      <c r="C8">
+        <v>71</v>
+      </c>
+      <c r="D8">
+        <v>78</v>
+      </c>
       <c r="E8">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>148.17222222222222</v>
       </c>
       <c r="F8">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>181.04999999999998</v>
       </c>
       <c r="G8">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>198.9</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>290</v>
+      </c>
+      <c r="C9">
+        <v>32</v>
+      </c>
+      <c r="D9">
+        <v>89</v>
+      </c>
       <c r="E9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>144.19444444444446</v>
       </c>
       <c r="F9">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>81.600000000000009</v>
       </c>
       <c r="G9">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>226.95000000000002</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>300</v>
+      </c>
+      <c r="C10">
+        <v>58</v>
+      </c>
+      <c r="D10">
+        <v>88</v>
+      </c>
       <c r="E10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>149.16666666666669</v>
       </c>
       <c r="F10">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>147.89999999999998</v>
       </c>
       <c r="G10">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>224.4</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>29</v>
+      </c>
+      <c r="C11">
+        <v>91</v>
+      </c>
+      <c r="D11">
+        <v>92</v>
+      </c>
       <c r="E11">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>14.419444444444446</v>
       </c>
       <c r="F11">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>232.05</v>
       </c>
       <c r="G11">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>234.60000000000002</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>26</v>
+      </c>
+      <c r="C12">
+        <v>43</v>
+      </c>
+      <c r="D12">
+        <v>93</v>
+      </c>
       <c r="E12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>12.927777777777777</v>
       </c>
       <c r="F12">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>109.64999999999999</v>
       </c>
       <c r="G12">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>237.15</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13">
+        <v>38</v>
+      </c>
+      <c r="C13">
+        <v>77</v>
+      </c>
+      <c r="D13">
+        <v>91</v>
+      </c>
       <c r="E13">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>18.894444444444446</v>
       </c>
       <c r="F13">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>196.35</v>
       </c>
       <c r="G13">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>232.05</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>9</v>
@@ -722,6 +809,9 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
+      <c r="D14">
+        <v>50</v>
+      </c>
       <c r="E14">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -732,7 +822,7 @@
       </c>
       <c r="G14">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>127.5</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>9</v>
@@ -740,6 +830,9 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
+      <c r="D15" t="s">
+        <v>18</v>
+      </c>
       <c r="E15">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -748,9 +841,9 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G15">
+      <c r="G15" t="e">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>#VALUE!</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>9</v>

</xml_diff>